<commit_message>
feat: add data validation to grade and student templates
</commit_message>
<xml_diff>
--- a/public/template/grade.xlsx
+++ b/public/template/grade.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aonro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\inu-garden\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BE14FB-9BCA-4E21-B6ED-3CCD57AC7FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DAF181B-CD8D-4FFE-8C0F-494B0F1BE58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{35AFC8FD-4AD2-4C44-BA1D-98EF137A88E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{35AFC8FD-4AD2-4C44-BA1D-98EF137A88E4}"/>
   </bookViews>
   <sheets>
     <sheet name="grade" sheetId="1" r:id="rId1"/>
@@ -58,13 +58,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Aptos Narrow"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -620,17 +620,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DDDC60B-8279-4056-9BFF-54022537842C}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" customWidth="1"/>
-    <col min="6" max="6" width="19.36328125" customWidth="1"/>
+    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="6" max="6" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -644,7 +644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>60000000000</v>
       </c>
@@ -655,10 +655,10 @@
         <v>2025</v>
       </c>
       <c r="F2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>60000000000</v>
       </c>
@@ -666,23 +666,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{B9EA261F-B559-4C7D-B49E-F04441CBA1DE}">
+      <formula1>"1,2,S"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>